<commit_message>
minor changes on formatting and adding micro-averages for F-scores
</commit_message>
<xml_diff>
--- a/docs/IAA_scores/4_FScores_entities_perPaper.xlsx
+++ b/docs/IAA_scores/4_FScores_entities_perPaper.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="58">
   <si>
     <t>PMID</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>C2 vs C3</t>
+  </si>
+  <si>
+    <t>Avrg</t>
   </si>
   <si>
     <t>PMC1955446</t>
@@ -402,8 +405,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -425,10 +428,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.86096256684492</v>
@@ -446,7 +452,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.652631578947368</v>
@@ -464,7 +470,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.916540212443096</v>
@@ -482,7 +488,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.726114649681529</v>
@@ -500,7 +506,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.825688073394495</v>
@@ -518,7 +524,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.64327485380117</v>
@@ -536,7 +542,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.408866995073892</v>
@@ -554,7 +560,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0.787037037037037</v>
@@ -572,7 +578,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0.661077844311377</v>
@@ -590,7 +596,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.648752399232246</v>
@@ -608,7 +614,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.726050420168067</v>
@@ -626,7 +632,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.653658536585366</v>
@@ -644,7 +650,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.662068965517241</v>
@@ -662,7 +668,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.752293577981651</v>
@@ -680,7 +686,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.541666666666667</v>
@@ -698,7 +704,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.576923076923077</v>
@@ -716,7 +722,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.47682119205298</v>
@@ -734,7 +740,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.669291338582677</v>
@@ -752,7 +758,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.713780918727915</v>
@@ -770,7 +776,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0.547140649149923</v>
@@ -788,7 +794,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0.807547169811321</v>
@@ -806,7 +812,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0.61271676300578</v>
@@ -824,7 +830,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>0.688775510204082</v>
@@ -842,7 +848,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0.647382920110193</v>
@@ -860,7 +866,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0.784810126582278</v>
@@ -878,7 +884,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>0.710359408033827</v>
@@ -896,7 +902,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>0.477211796246649</v>
@@ -914,7 +920,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>0.634050880626223</v>
@@ -932,7 +938,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>0.786155747836836</v>
@@ -950,7 +956,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>0.76056338028169</v>
@@ -968,7 +974,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>0.854736842105263</v>
@@ -986,7 +992,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>0.624454148471616</v>
@@ -1004,7 +1010,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>0.842650103519669</v>
@@ -1022,7 +1028,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>0.838235294117647</v>
@@ -1040,7 +1046,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>0.610086100861009</v>
@@ -1058,7 +1064,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>0.780141843971631</v>
@@ -1076,7 +1082,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>0.725274725274725</v>
@@ -1094,7 +1100,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>0.552831783601014</v>
@@ -1112,7 +1118,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>0.770642201834862</v>
@@ -1130,7 +1136,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>0.846560846560847</v>
@@ -1148,7 +1154,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>0.713625866050808</v>
@@ -1166,7 +1172,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>0.714606741573034</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>0.551301684532925</v>
@@ -1202,7 +1208,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>0.850174216027875</v>
@@ -1220,7 +1226,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>0.702179176755448</v>
@@ -1238,7 +1244,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>0.791180285343709</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0.693467336683417</v>
@@ -1274,7 +1280,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>0.611801242236025</v>
@@ -1292,7 +1298,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>0.740983606557377</v>
@@ -1310,7 +1316,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>0.617059891107078</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="n">
         <f aca="false">SUM(A2:B51)/50</f>
@@ -1342,22 +1348,51 @@
         <f aca="false">SUM(D2:D51)/50</f>
         <v>0.656931885531828</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <f aca="false">SUM(B53:D53)/3</f>
         <v>0.714743229889313</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.796</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">SUM(B54:D54)/3</f>
+        <v>0.717</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <f aca="false">(SUM(B2:B51) - B39 - B42 )/48</f>
+        <v>0.698453157154078</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <f aca="false">(SUM(C2:C51) - C39 - C42 )/48</f>
+        <v>0.792526484215388</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">(SUM(D2:D51) - D39 - D42 )/48</f>
+        <v>0.658287567529035</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">SUM(B56:D56)/3</f>
+        <v>0.716422402966167</v>
       </c>
     </row>
   </sheetData>
@@ -1383,8 +1418,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1393,7 +1428,7 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1406,10 +1441,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.949197860962567</v>
@@ -1427,7 +1465,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.963157894736842</v>
@@ -1445,7 +1483,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.955993930197269</v>
@@ -1463,7 +1501,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.885350318471338</v>
@@ -1481,7 +1519,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.91131498470948</v>
@@ -1499,7 +1537,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.807017543859649</v>
@@ -1517,7 +1555,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.822660098522167</v>
@@ -1535,7 +1573,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0.856481481481482</v>
@@ -1553,7 +1591,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0.752095808383234</v>
@@ -1571,7 +1609,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.852207293666027</v>
@@ -1589,7 +1627,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.884033613445378</v>
@@ -1607,7 +1645,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.770731707317073</v>
@@ -1625,7 +1663,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.841379310344828</v>
@@ -1643,7 +1681,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.788990825688073</v>
@@ -1661,7 +1699,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.645833333333333</v>
@@ -1679,7 +1717,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.661538461538462</v>
@@ -1697,7 +1735,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.847682119205298</v>
@@ -1715,7 +1753,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.89238845144357</v>
@@ -1733,7 +1771,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.872791519434629</v>
@@ -1751,7 +1789,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0.884080370942813</v>
@@ -1769,7 +1807,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0.830188679245283</v>
@@ -1787,7 +1825,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0.878612716763006</v>
@@ -1805,7 +1843,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>0.811224489795918</v>
@@ -1823,7 +1861,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0.845730027548209</v>
@@ -1841,7 +1879,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0.815189873417721</v>
@@ -1859,7 +1897,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>0.765327695560254</v>
@@ -1877,7 +1915,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>0.648793565683646</v>
@@ -1895,7 +1933,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>0.692759295499021</v>
@@ -1913,7 +1951,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>0.875154511742892</v>
@@ -1931,7 +1969,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>0.807511737089202</v>
@@ -1949,7 +1987,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>0.892631578947368</v>
@@ -1967,7 +2005,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>0.759825327510917</v>
@@ -1985,7 +2023,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>0.910973084886128</v>
@@ -2003,7 +2041,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>0.860294117647059</v>
@@ -2021,7 +2059,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>0.826568265682657</v>
@@ -2039,7 +2077,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>0.851063829787234</v>
@@ -2057,7 +2095,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>0.868131868131868</v>
@@ -2075,7 +2113,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>0.762468300929839</v>
@@ -2093,7 +2131,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>0.840366972477064</v>
@@ -2111,7 +2149,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>0.867724867724868</v>
@@ -2129,7 +2167,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>0.863741339491917</v>
@@ -2147,7 +2185,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>0.91685393258427</v>
@@ -2165,7 +2203,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>0.719754977029097</v>
@@ -2183,7 +2221,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>0.895470383275261</v>
@@ -2201,7 +2239,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>0.75544794188862</v>
@@ -2219,7 +2257,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>0.809338521400778</v>
@@ -2237,7 +2275,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0.798994974874372</v>
@@ -2255,7 +2293,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>0.804347826086956</v>
@@ -2273,7 +2311,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>0.79344262295082</v>
@@ -2291,7 +2329,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>0.693284936479129</v>
@@ -2307,9 +2345,9 @@
         <v>0.773258141174897</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="n">
         <f aca="false">SUM(B2:B51)/50</f>
@@ -2323,22 +2361,51 @@
         <f aca="false">SUM(D2:D51)/50</f>
         <v>0.812969179705557</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <f aca="false">SUM(B53:D53)/3</f>
         <v>0.83578265285015</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.874</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">SUM(B54:D54)/3</f>
+        <v>0.842666666666667</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <f aca="false">(SUM(B2:B51) - B39 - B42 )/48</f>
+        <v>0.82666532394569</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <f aca="false">(SUM(C2:C51) - C39 - C42 )/48</f>
+        <v>0.869637344399862</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">(SUM(D2:D51) - D39 - D42 )/48</f>
+        <v>0.810728013428253</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">SUM(B56:D56)/3</f>
+        <v>0.835676893924602</v>
       </c>
     </row>
   </sheetData>
@@ -2364,8 +2431,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2374,7 +2441,7 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2387,10 +2454,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.866310160427807</v>
@@ -2408,7 +2478,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.663157894736842</v>
@@ -2426,7 +2496,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.916540212443096</v>
@@ -2444,7 +2514,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.764331210191083</v>
@@ -2462,7 +2532,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.831804281345566</v>
@@ -2480,7 +2550,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.672514619883041</v>
@@ -2498,7 +2568,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.41871921182266</v>
@@ -2516,7 +2586,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0.800925925925926</v>
@@ -2534,7 +2604,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0.747305389221557</v>
@@ -2552,7 +2622,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.683301343570058</v>
@@ -2570,7 +2640,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.742857142857143</v>
@@ -2588,7 +2658,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.682926829268293</v>
@@ -2606,7 +2676,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.717241379310345</v>
@@ -2624,7 +2694,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.807339449541284</v>
@@ -2642,7 +2712,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.5625</v>
@@ -2660,7 +2730,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.588461538461538</v>
@@ -2678,7 +2748,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.494481236203091</v>
@@ -2696,7 +2766,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.692913385826772</v>
@@ -2714,7 +2784,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.734982332155477</v>
@@ -2732,7 +2802,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0.553323029366306</v>
@@ -2750,7 +2820,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0.807547169811321</v>
@@ -2768,7 +2838,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0.61271676300578</v>
@@ -2786,7 +2856,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>0.73469387755102</v>
@@ -2804,7 +2874,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0.707988980716254</v>
@@ -2822,7 +2892,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0.80506329113924</v>
@@ -2840,7 +2910,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>0.875264270613108</v>
@@ -2858,7 +2928,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>0.487935656836461</v>
@@ -2876,7 +2946,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>0.73972602739726</v>
@@ -2894,7 +2964,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>0.84796044499382</v>
@@ -2912,7 +2982,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>0.788732394366197</v>
@@ -2930,7 +3000,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>0.884210526315789</v>
@@ -2948,7 +3018,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>0.65938864628821</v>
@@ -2966,7 +3036,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>0.857142857142857</v>
@@ -2984,7 +3054,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>0.889705882352941</v>
@@ -3002,7 +3072,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>0.619926199261993</v>
@@ -3020,7 +3090,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>0.836879432624114</v>
@@ -3038,7 +3108,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>0.754578754578755</v>
@@ -3056,7 +3126,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>0.613693998309383</v>
@@ -3074,7 +3144,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>0.836697247706422</v>
@@ -3092,7 +3162,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>0.899470899470899</v>
@@ -3110,7 +3180,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>0.74364896073903</v>
@@ -3128,7 +3198,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>0.728089887640449</v>
@@ -3146,7 +3216,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>0.64624808575804</v>
@@ -3164,7 +3234,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>0.860627177700348</v>
@@ -3182,7 +3252,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>0.774818401937046</v>
@@ -3200,7 +3270,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>0.954604409857328</v>
@@ -3218,7 +3288,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0.723618090452261</v>
@@ -3236,7 +3306,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>0.664596273291926</v>
@@ -3254,7 +3324,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>0.859016393442623</v>
@@ -3272,7 +3342,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>0.682395644283122</v>
@@ -3293,9 +3363,9 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="n">
         <f aca="false">SUM(B2:B51)/50</f>
@@ -3309,22 +3379,51 @@
         <f aca="false">SUM(D2:D51)/50</f>
         <v>0.699471536214084</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <f aca="false">SUM(B53:D53)/3</f>
         <v>0.757516088663682</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.842</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.701</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">SUM(B54:D54)/3</f>
+        <v>0.760333333333333</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <f aca="false">(SUM(B2:B51) - B39 - B42 )/48</f>
+        <v>0.739199588731114</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <f aca="false">(SUM(C2:C51) - C39 - C42 )/48</f>
+        <v>0.835356343026479</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">(SUM(D2:D51) - D39 - D42 )/48</f>
+        <v>0.701194345837689</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">SUM(B56:D56)/3</f>
+        <v>0.758583425865094</v>
       </c>
     </row>
   </sheetData>
@@ -3350,8 +3449,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3373,10 +3472,13 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.954545454545455</v>
@@ -3394,7 +3496,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.973684210526316</v>
@@ -3412,7 +3514,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.955993930197269</v>
@@ -3430,7 +3532,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.929936305732484</v>
@@ -3448,7 +3550,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.960244648318043</v>
@@ -3466,7 +3568,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.842105263157895</v>
@@ -3484,7 +3586,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.83743842364532</v>
@@ -3502,7 +3604,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0.916666666666667</v>
@@ -3520,7 +3622,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0.943712574850299</v>
@@ -3538,7 +3640,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.9021113243762</v>
@@ -3556,7 +3658,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.927731092436975</v>
@@ -3574,7 +3676,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.839024390243902</v>
@@ -3592,7 +3694,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.901149425287356</v>
@@ -3610,7 +3712,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.844036697247706</v>
@@ -3628,7 +3730,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.739583333333333</v>
@@ -3646,7 +3748,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.688461538461538</v>
@@ -3664,7 +3766,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.944812362030905</v>
@@ -3682,7 +3784,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.934383202099738</v>
@@ -3700,7 +3802,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.915194346289753</v>
@@ -3718,7 +3820,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0.899536321483771</v>
@@ -3736,7 +3838,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0.830188679245283</v>
@@ -3754,7 +3856,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0.901734104046243</v>
@@ -3772,7 +3874,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>0.887755102040816</v>
@@ -3790,7 +3892,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0.950413223140496</v>
@@ -3808,7 +3910,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0.855696202531646</v>
@@ -3826,7 +3928,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>0.938689217758985</v>
@@ -3844,7 +3946,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>0.675603217158177</v>
@@ -3862,7 +3964,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>0.806262230919765</v>
@@ -3880,7 +3982,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>0.941903584672435</v>
@@ -3898,7 +4000,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>0.868544600938967</v>
@@ -3916,7 +4018,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>0.930526315789474</v>
@@ -3934,7 +4036,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>0.807860262008734</v>
@@ -3952,7 +4054,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>0.929606625258799</v>
@@ -3970,7 +4072,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>0.911764705882353</v>
@@ -3988,7 +4090,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>0.885608856088561</v>
@@ -4006,7 +4108,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>0.921985815602837</v>
@@ -4024,7 +4126,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>0.941391941391941</v>
@@ -4042,7 +4144,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>0.943364327979713</v>
@@ -4060,7 +4162,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>0.924770642201835</v>
@@ -4078,7 +4180,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>0.952380952380952</v>
@@ -4096,7 +4198,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>0.930715935334873</v>
@@ -4114,7 +4216,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>0.934831460674157</v>
@@ -4132,7 +4234,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>0.848392036753446</v>
@@ -4150,7 +4252,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>0.947735191637631</v>
@@ -4168,7 +4270,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>0.861985472154964</v>
@@ -4186,7 +4288,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>0.977950713359273</v>
@@ -4204,7 +4306,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0.919597989949749</v>
@@ -4222,7 +4324,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>0.916149068322981</v>
@@ -4240,7 +4342,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>0.924590163934426</v>
@@ -4258,7 +4360,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>0.831215970961888</v>
@@ -4274,9 +4376,9 @@
         <v>0.877820630904318</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="n">
         <f aca="false">SUM(B2:B51)/50</f>
@@ -4290,22 +4392,51 @@
         <f aca="false">SUM(D2:D51)/50</f>
         <v>0.887826799761078</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <f aca="false">SUM(B53:D53)/3</f>
         <v>0.905420976952184</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.904</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.939</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.897</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">SUM(B54:D54)/3</f>
+        <v>0.913333333333333</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <f aca="false">(SUM(B2:B51) - B39 - B42 )/48</f>
+        <v>0.893239288702869</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <f aca="false">(SUM(C2:C51) - C39 - C42 )/48</f>
+        <v>0.932547457444104</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">(SUM(D2:D51) - D39 - D42 )/48</f>
+        <v>0.88553958110983</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">SUM(B56:D56)/3</f>
+        <v>0.903775442418934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>